<commit_message>
Ajuste practica frijoles y script simulación
</commit_message>
<xml_diff>
--- a/Calendario-EP-2026-2.xlsx
+++ b/Calendario-EP-2026-2.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Asistencia" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="13">
   <si>
     <t xml:space="preserve">Profesor</t>
   </si>
@@ -35,6 +36,30 @@
   </si>
   <si>
     <t xml:space="preserve">Rusby</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nombre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ana Cristina Uc Canela</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xiadani Briones García</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jamil Jassiel Hernández Enríquez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Casandra Gallardo Badillo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Renata Flores García</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pablo Villanueva Valdez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rodrigo Chan Catzim</t>
   </si>
 </sst>
 </file>
@@ -135,7 +160,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -161,6 +186,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -243,11 +272,11 @@
   </sheetPr>
   <dimension ref="A1:C97"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.94"/>
   </cols>
@@ -796,4 +825,252 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:J8"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.72"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="7" t="n">
+        <v>46056</v>
+      </c>
+      <c r="C1" s="7" t="n">
+        <v>46059</v>
+      </c>
+      <c r="D1" s="7" t="n">
+        <f aca="false">B1+7</f>
+        <v>46063</v>
+      </c>
+      <c r="E1" s="7" t="n">
+        <f aca="false">C1+7</f>
+        <v>46066</v>
+      </c>
+      <c r="F1" s="7" t="n">
+        <f aca="false">D1+7</f>
+        <v>46070</v>
+      </c>
+      <c r="G1" s="7" t="n">
+        <f aca="false">E1+7</f>
+        <v>46073</v>
+      </c>
+      <c r="H1" s="7" t="n">
+        <f aca="false">F1+7</f>
+        <v>46077</v>
+      </c>
+      <c r="I1" s="7" t="n">
+        <f aca="false">G1+7</f>
+        <v>46080</v>
+      </c>
+      <c r="J1" s="7" t="n">
+        <f aca="false">H1+7</f>
+        <v>46084</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>